<commit_message>
Update: $(Get-Date -Format 'yyyy-MM-dd')
</commit_message>
<xml_diff>
--- a/Piano HPC.xlsx
+++ b/Piano HPC.xlsx
@@ -704,13 +704,13 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="none"/>
+      <right style="none"/>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -741,13 +741,13 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="none"/>
+      <right style="none"/>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -3037,7 +3037,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="13" operator="between" id="{00E400F5-008D-4968-A6D6-00A700BB0067}">
+          <x14:cfRule type="cellIs" priority="13" operator="between" id="{008E008E-00EF-4B22-BDC6-00F100D900AD}">
             <xm:f>45</xm:f>
             <xm:f>65</xm:f>
             <x14:dxf>
@@ -3055,7 +3055,7 @@
           <xm:sqref>E28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="12" operator="between" id="{00A8005F-0094-4810-A357-001400560090}">
+          <x14:cfRule type="cellIs" priority="12" operator="between" id="{00480071-006E-49DF-A6D5-005100FA0028}">
             <xm:f>30</xm:f>
             <xm:f>45</xm:f>
             <x14:dxf>
@@ -3073,7 +3073,7 @@
           <xm:sqref>E29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" operator="between" id="{007600B7-00C3-43BC-98EC-000000D300BF}">
+          <x14:cfRule type="cellIs" priority="11" operator="between" id="{006F009B-0006-4B4A-87A9-007200F80051}">
             <xm:f>10</xm:f>
             <xm:f>20</xm:f>
             <x14:dxf>
@@ -3091,7 +3091,7 @@
           <xm:sqref>E30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="10" operator="lessThan" id="{00120091-0067-4F28-A0D9-00D7008D0055}">
+          <x14:cfRule type="cellIs" priority="10" operator="lessThan" id="{005400C8-00F9-4378-ADB5-00AB0089006A}">
             <xm:f>45</xm:f>
             <x14:dxf>
               <font>
@@ -3108,7 +3108,7 @@
           <xm:sqref>E28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" operator="greaterThan" id="{00220035-0094-4C23-8A03-007400670088}">
+          <x14:cfRule type="cellIs" priority="9" operator="greaterThan" id="{00600053-00FF-4B01-9A4B-00B8009A00F9}">
             <xm:f>65</xm:f>
             <x14:dxf>
               <font>
@@ -3125,7 +3125,7 @@
           <xm:sqref>E28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="lessThan" id="{00B20020-00A1-4C0F-A372-00AC004300E1}">
+          <x14:cfRule type="cellIs" priority="8" operator="lessThan" id="{008D00C0-00C0-4583-9B0B-003800CC004A}">
             <xm:f>30</xm:f>
             <x14:dxf>
               <font>
@@ -3142,7 +3142,7 @@
           <xm:sqref>E29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="greaterThan" id="{00B30081-00A7-4063-96D5-00C4008C00BC}">
+          <x14:cfRule type="cellIs" priority="7" operator="greaterThan" id="{00EB0033-005A-481D-B267-003000F200EA}">
             <xm:f>45</xm:f>
             <x14:dxf>
               <font>
@@ -3159,7 +3159,7 @@
           <xm:sqref>E29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="lessThan" id="{007700BE-0005-4B2C-92FE-00F600AD00CB}">
+          <x14:cfRule type="cellIs" priority="6" operator="lessThan" id="{001C00F6-00E1-4FF5-902C-00870094002D}">
             <xm:f>10</xm:f>
             <x14:dxf>
               <font>
@@ -3176,7 +3176,7 @@
           <xm:sqref>E30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="greaterThan" id="{003600ED-00DF-4F87-8662-00F100970093}">
+          <x14:cfRule type="cellIs" priority="5" operator="greaterThan" id="{00D800F7-00DA-48B3-99F5-0088006F00AA}">
             <xm:f>20</xm:f>
             <x14:dxf>
               <font>
@@ -3193,7 +3193,7 @@
           <xm:sqref>E30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{008D005B-009A-4229-A99B-0056003F00ED}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{006A0047-00BF-4303-83B4-006300F200BA}">
             <xm:f>120</xm:f>
             <x14:dxf>
               <font>
@@ -3210,7 +3210,7 @@
           <xm:sqref>E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="lessThan" id="{00FA0008-0061-49D8-99E4-003B001E0086}">
+          <x14:cfRule type="cellIs" priority="3" operator="lessThan" id="{0031009C-007E-4B16-B82F-00AC00C200FC}">
             <xm:f>120</xm:f>
             <x14:dxf>
               <font>
@@ -3227,7 +3227,7 @@
           <xm:sqref>E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="greaterThan" id="{00610029-00A4-4FEF-83A4-00AC00B00060}">
+          <x14:cfRule type="cellIs" priority="2" operator="greaterThan" id="{002000D0-00FA-4F21-917E-00DA003700D4}">
             <xm:f>120</xm:f>
             <x14:dxf>
               <font>
@@ -3244,7 +3244,7 @@
           <xm:sqref>E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{008A00A5-0093-40DE-9CDB-002500F5004E}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{003E0060-0088-45DD-A18D-00C900DD00E7}">
             <xm:f>20</xm:f>
             <x14:dxf>
               <font>
@@ -3356,7 +3356,6 @@
       </c>
       <c r="G4" s="88"/>
       <c r="H4" s="92"/>
-      <c r="I4"/>
     </row>
     <row r="5" ht="14.25">
       <c r="H5" s="92"/>
@@ -3529,19 +3528,19 @@
       <c r="H14" s="92"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="97">
+      <c r="B15" s="49">
         <v>2</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="97">
+      <c r="E15" s="49">
         <v>5</v>
       </c>
       <c r="F15" s="49"/>
@@ -3588,11 +3587,7 @@
       <c r="G17" s="96"/>
       <c r="H17" s="92"/>
     </row>
-    <row r="18" ht="14.25">
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-    </row>
+    <row r="18" ht="14.25"/>
     <row r="19" ht="14.25">
       <c r="A19" s="22" t="s">
         <v>8</v>
@@ -3725,7 +3720,6 @@
       <c r="E25" s="42">
         <v>5</v>
       </c>
-      <c r="F25"/>
       <c r="G25" s="88"/>
       <c r="H25" s="98"/>
     </row>

</xml_diff>